<commit_message>
Updating WK2 HW Update
</commit_message>
<xml_diff>
--- a/Section2/ExcelHomework.xlsx
+++ b/Section2/ExcelHomework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casil\Documents\Savvy Coders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE52BECD-C545-42F6-A7EB-52EE19D67318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D38F9F-BE4E-4E2D-8D0C-9DD8D649E57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13200" yWindow="0" windowWidth="30105" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="3300" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Payments" sheetId="4" r:id="rId1"/>
@@ -20,13 +20,13 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="170">
   <si>
     <t>Expenses</t>
   </si>
@@ -637,7 +637,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -688,115 +688,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="52">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <alignment wrapText="1"/>
     </dxf>
@@ -1089,40 +987,122 @@
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -1189,11 +1169,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Payments!$C$3</c:f>
+              <c:f>Payments!$B$3:$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Total</c:v>
+                  <c:v>B1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1209,63 +1189,147 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>Payments!$A$4:$B$10</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>B1</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>B2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>PC</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>B1</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>B2</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>PC</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Jan</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Feb</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+            <c:strRef>
+              <c:f>Payments!$A$5:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Payments!$C$4:$C$10</c:f>
+              <c:f>Payments!$B$5:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>30270.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>34624</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2596-4316-9293-3BC92E3085BF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Payments!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>B2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Payments!$A$5:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Payments!$C$5:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C0A8-47CC-8B33-79082BEBB3A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Payments!$D$3:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Payments!$A$5:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Payments!$D$5:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
                   <c:v>-4</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>34624</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
@@ -1273,7 +1337,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2596-4316-9293-3BC92E3085BF}"/>
+              <c16:uniqueId val="{00000001-C0A8-47CC-8B33-79082BEBB3A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4137,16 +4201,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>510778</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>375045</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1253625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>10300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1446610</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1432374</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>59530</xdr:rowOff>
+      <xdr:rowOff>66260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11850,8 +11914,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{24C77926-4843-4AE2-BC2B-DFF4CA7282CD}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:C10" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{24C77926-4843-4AE2-BC2B-DFF4CA7282CD}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField compact="0" numFmtId="14" outline="0" showAll="0">
       <extLst>
@@ -11967,7 +12031,7 @@
         </ext>
       </extLst>
     </pivotField>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0">
       <items count="4">
         <item x="0"/>
         <item x="1"/>
@@ -12039,49 +12103,48 @@
       </extLst>
     </pivotField>
   </pivotFields>
-  <rowFields count="2">
+  <rowFields count="1">
     <field x="8"/>
-    <field x="6"/>
   </rowFields>
-  <rowItems count="7">
+  <rowItems count="3">
     <i>
       <x v="1"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
     </i>
     <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
       <x v="2"/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="6"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="8" baseItem="1" numFmtId="8"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="51">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="16">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -12091,12 +12154,36 @@
       </pivotArea>
     </format>
   </formats>
-  <chartFormats count="1">
+  <chartFormats count="3">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -12126,18 +12213,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77EA7A96-A625-4CD7-A09C-F5CF2DA5553C}" name="ExpTbl" displayName="ExpTbl" ref="A2:I210" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77EA7A96-A625-4CD7-A09C-F5CF2DA5553C}" name="ExpTbl" displayName="ExpTbl" ref="A2:I210" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
   <autoFilter ref="A2:I210" xr:uid="{77EA7A96-A625-4CD7-A09C-F5CF2DA5553C}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0F5BF222-85C4-4AC8-A471-CA939CE36E4C}" name="Document Date" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{517CCC46-72D3-4C4C-8508-4BFA949B5A1F}" name="Supplier" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{FC228CD2-8606-4A9D-931C-CF4FA8F4DFE4}" name="Reference" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{1089A22A-8C4F-4D7A-922E-A80E21BD6E9B}" name="Description" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{CA4CEDF3-B2C5-47D9-A6A1-2B327965F8AC}" name="Tax Inclusive Amount" dataDxfId="40" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{3CA136A0-D51E-433E-92AB-63D7DB8CB4CC}" name="Tax Code" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{161FC37A-160D-478A-98E7-22C05E0C768C}" name="Bank Code" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{045980F3-D3FF-4E49-9F9D-F89EC6C31E3C}" name="Account Code" dataDxfId="37"/>
-    <tableColumn id="9" xr3:uid="{D11E8517-5C8B-4233-9EC1-A08331AB8CA6}" name="Payment Date" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{0F5BF222-85C4-4AC8-A471-CA939CE36E4C}" name="Document Date" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{517CCC46-72D3-4C4C-8508-4BFA949B5A1F}" name="Supplier" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{FC228CD2-8606-4A9D-931C-CF4FA8F4DFE4}" name="Reference" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{1089A22A-8C4F-4D7A-922E-A80E21BD6E9B}" name="Description" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{CA4CEDF3-B2C5-47D9-A6A1-2B327965F8AC}" name="Tax Inclusive Amount" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{3CA136A0-D51E-433E-92AB-63D7DB8CB4CC}" name="Tax Code" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{161FC37A-160D-478A-98E7-22C05E0C768C}" name="Bank Code" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{045980F3-D3FF-4E49-9F9D-F89EC6C31E3C}" name="Account Code" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{D11E8517-5C8B-4233-9EC1-A08331AB8CA6}" name="Payment Date" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12440,105 +12527,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E3ADE1-28B5-48F7-96DE-0815846F3FFA}">
-  <dimension ref="A3:C10"/>
+  <dimension ref="A3:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="72" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>8</v>
+        <v>166</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>168</v>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="25">
-        <v>30270.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>168</v>
       </c>
-      <c r="B5" t="s">
-        <v>31</v>
+      <c r="B5" s="25">
+        <v>30270.25</v>
       </c>
       <c r="C5" s="25">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="25">
+        <v>-4</v>
+      </c>
+      <c r="E5" s="25">
+        <v>30301.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
+        <v>169</v>
+      </c>
+      <c r="B6" s="25">
+        <v>34624</v>
       </c>
       <c r="C6" s="25">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="D6" s="25">
+        <v>5</v>
+      </c>
+      <c r="E6" s="25">
+        <v>34664</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
+        <v>167</v>
+      </c>
+      <c r="B7" s="25">
+        <v>64894.25</v>
       </c>
       <c r="C7" s="25">
-        <v>34624</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>169</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="25">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>167</v>
-      </c>
-      <c r="C10" s="25">
+        <v>70</v>
+      </c>
+      <c r="D7" s="25">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25">
         <v>64965.25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating HW WK2 Pivot Table
</commit_message>
<xml_diff>
--- a/Section2/ExcelHomework.xlsx
+++ b/Section2/ExcelHomework.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casil\Documents\Savvy Coders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casil\Code\SavvyCoders\Homework\Section2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D38F9F-BE4E-4E2D-8D0C-9DD8D649E57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53F2FD1-1310-4A18-A16F-DB45F9D9F160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="3300" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="170">
   <si>
     <t>Expenses</t>
   </si>
@@ -637,7 +637,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -688,6 +688,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -987,6 +990,36 @@
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:pivotFmts>
       <c:pivotFmt>
@@ -1157,6 +1190,62 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -1169,11 +1258,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Payments!$B$3:$B$4</c:f>
+              <c:f>Payments!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>B1</c:v>
+                  <c:v>Total</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1189,30 +1278,64 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Payments!$A$5:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>Payments!$A$4:$B$10</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>B1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>B2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>B1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>B2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>PC</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Payments!$B$5:$B$7</c:f>
+              <c:f>Payments!$C$4:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>30270.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>34624</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1220,124 +1343,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2596-4316-9293-3BC92E3085BF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Payments!$C$3:$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>B2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Payments!$A$5:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Payments!$C$5:$C$7</c:f>
-              <c:numCache>
-                <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>35</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C0A8-47CC-8B33-79082BEBB3A7}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Payments!$D$3:$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Payments!$A$5:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Payments!$D$5:$D$7</c:f>
-              <c:numCache>
-                <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C0A8-47CC-8B33-79082BEBB3A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -11915,7 +11920,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{24C77926-4843-4AE2-BC2B-DFF4CA7282CD}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A3:C10" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="11">
     <pivotField compact="0" numFmtId="14" outline="0" showAll="0">
       <extLst>
@@ -12031,7 +12036,7 @@
         </ext>
       </extLst>
     </pivotField>
-    <pivotField axis="axisCol" compact="0" outline="0" showAll="0">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
       <items count="4">
         <item x="0"/>
         <item x="1"/>
@@ -12103,36 +12108,37 @@
       </extLst>
     </pivotField>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="2">
     <field x="8"/>
+    <field x="6"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="7">
     <i>
       <x v="1"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
     </i>
     <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
       <x v="2"/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
-  <colFields count="1">
-    <field x="6"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="8" baseItem="1" numFmtId="8"/>
@@ -12154,7 +12160,7 @@
       </pivotArea>
     </format>
   </formats>
-  <chartFormats count="3">
+  <chartFormats count="4">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -12184,6 +12190,18 @@
           </reference>
           <reference field="6" count="1" selected="0">
             <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
@@ -12527,10 +12545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E3ADE1-28B5-48F7-96DE-0815846F3FFA}">
-  <dimension ref="A3:E7"/>
+  <dimension ref="A3:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12540,79 +12558,88 @@
     <col min="73" max="73" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>166</v>
+        <v>8</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>8</v>
+      <c r="C3" s="26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>168</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="25">
+        <v>30270.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>168</v>
       </c>
-      <c r="B5" s="25">
-        <v>30270.25</v>
+      <c r="B5" t="s">
+        <v>31</v>
       </c>
       <c r="C5" s="25">
         <v>35</v>
       </c>
-      <c r="D5" s="25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="25">
         <v>-4</v>
       </c>
-      <c r="E5" s="25">
-        <v>30301.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>169</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="25">
         <v>34624</v>
       </c>
-      <c r="C6" s="25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="25">
         <v>35</v>
       </c>
-      <c r="D6" s="25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="25">
         <v>5</v>
       </c>
-      <c r="E6" s="25">
-        <v>34664</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>167</v>
       </c>
-      <c r="B7" s="25">
-        <v>64894.25</v>
-      </c>
-      <c r="C7" s="25">
-        <v>70</v>
-      </c>
-      <c r="D7" s="25">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25">
+      <c r="C10" s="25">
         <v>64965.25</v>
       </c>
     </row>

</xml_diff>